<commit_message>
Resultados gerados com o arquivo csv
</commit_message>
<xml_diff>
--- a/Resultados/resultados.xlsx
+++ b/Resultados/resultados.xlsx
@@ -32,9 +32,6 @@
     <t>Nome das Bases de dados</t>
   </si>
   <si>
-    <t>Valor de G com K2 aleatório</t>
-  </si>
-  <si>
     <t>Valor de G com Boruta + K2</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>Sachs</t>
+  </si>
+  <si>
+    <t>Valor de G com K2 aleatório (Média de 10x)</t>
   </si>
 </sst>
 </file>
@@ -92,7 +92,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -115,22 +115,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -416,134 +471,144 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:I3"/>
+      <selection activeCell="D4" sqref="D4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="G9:I9"/>
@@ -555,18 +620,8 @@
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
   </mergeCells>

</xml_diff>

<commit_message>
Resultados de ordenação com Pearson e Spearman
</commit_message>
<xml_diff>
--- a/Resultados/resultados.xlsx
+++ b/Resultados/resultados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Relatório dos dados obtidos com as interações</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Valor de G com K2 aleatório (Média de 10x)</t>
+  </si>
+  <si>
+    <t>Valor de G com Pearson + K2</t>
+  </si>
+  <si>
+    <t>Valor de G com Spearman + K2</t>
   </si>
 </sst>
 </file>
@@ -64,9 +70,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="171" formatCode="0.000000000"/>
-    <numFmt numFmtId="172" formatCode="0.0000000000"/>
-    <numFmt numFmtId="175" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -97,7 +103,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -157,14 +163,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -174,13 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -195,19 +222,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -490,88 +517,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="9" width="8.88671875" style="1"/>
+    <col min="4" max="8" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+    </row>
+    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="3" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="15">
-        <v>-10.835108634727399</v>
-      </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6">
+        <v>-108351.086347274</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="12">
         <v>-107640.87088336601</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="19">
+        <v>-106584.24084760599</v>
+      </c>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="19">
+        <v>-106733.897947712</v>
+      </c>
+      <c r="N3" s="20"/>
+      <c r="O3" s="21"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="17">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7">
         <v>-22293.250145522499</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="14">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="4">
         <v>-22269.221900624801</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="19">
+        <v>-22281.743215127499</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="19">
+        <v>-22281.743215127499</v>
+      </c>
+      <c r="N4" s="20"/>
+      <c r="O4" s="21"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="8">
         <v>8493179607427180</v>
       </c>
@@ -582,78 +645,152 @@
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="J5" s="19"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="21"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="15">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6">
         <v>-99.421989636013805</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6">
         <v>-98.725036474119193</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="19">
+        <v>-98.725036474119193</v>
+      </c>
+      <c r="K6" s="20"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="19">
+        <v>-98.725036474119193</v>
+      </c>
+      <c r="N6" s="20"/>
+      <c r="O6" s="21"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="13">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="3">
         <v>-131959.73464283801</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
         <v>-48697.597856795997</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="19">
+        <v>-312176.87492872798</v>
+      </c>
+      <c r="K7" s="20"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="19">
+        <v>-309986.35200304398</v>
+      </c>
+      <c r="N7" s="20"/>
+      <c r="O7" s="21"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="13">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="3">
         <v>-327502.17691625102</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
         <v>-325468.98963063699</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="19">
+        <v>-325843.581118726</v>
+      </c>
+      <c r="K8" s="20"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="19">
+        <v>-325836.60571619001</v>
+      </c>
+      <c r="N8" s="20"/>
+      <c r="O8" s="21"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="14">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4">
         <v>-73154.396144125698</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4">
         <v>-72258.093905970905</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="K9" s="2"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="19">
+        <v>-72267.141452557</v>
+      </c>
+      <c r="K9" s="20"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="19">
+        <v>-72270.109038895098</v>
+      </c>
+      <c r="N9" s="20"/>
+      <c r="O9" s="21"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J13" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="41">
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="G9:I9"/>
@@ -669,16 +806,6 @@
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>